<commit_message>
Added and Updated some backlog
</commit_message>
<xml_diff>
--- a/Backlogs.xlsx
+++ b/Backlogs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>Backlog</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Pending</t>
   </si>
   <si>
-    <t>There should be a template for Login, Header and Footer</t>
-  </si>
-  <si>
     <t>There should be a template for User Profile</t>
   </si>
   <si>
@@ -58,6 +55,24 @@
   </si>
   <si>
     <t>DONE</t>
+  </si>
+  <si>
+    <t>There should be a template for Entity List</t>
+  </si>
+  <si>
+    <t>There should be a template for Entity Form</t>
+  </si>
+  <si>
+    <t>There should be a template for Toolbar</t>
+  </si>
+  <si>
+    <t>There should be a template for Login</t>
+  </si>
+  <si>
+    <t>There should be a template for Footer</t>
+  </si>
+  <si>
+    <t>There should be a template for  Header</t>
   </si>
 </sst>
 </file>
@@ -478,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,10 +531,10 @@
     </row>
     <row r="4" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -527,10 +542,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -538,17 +553,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>6</v>
@@ -556,12 +571,53 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
+    </row>
+    <row r="13" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Migrated From VSC to VS 2017 IDE.
- Included Identity for Authorization.
</commit_message>
<xml_diff>
--- a/Backlogs.xlsx
+++ b/Backlogs.xlsx
@@ -544,7 +544,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,7 +601,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -609,12 +609,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>4</v>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Dynamic Renderer for Web Links
</commit_message>
<xml_diff>
--- a/Backlogs.xlsx
+++ b/Backlogs.xlsx
@@ -544,7 +544,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,15 +585,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -613,8 +613,8 @@
       <c r="A8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>7</v>
+      <c r="B8" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated Backlogs and Read Me
</commit_message>
<xml_diff>
--- a/Backlogs.xlsx
+++ b/Backlogs.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Back-End" sheetId="1" r:id="rId1"/>
+    <sheet name="UI-UX" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
   <si>
     <t>Backlog</t>
   </si>
@@ -42,9 +43,6 @@
     <t>There should be a template for Navigation</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>DONE</t>
   </si>
   <si>
@@ -108,23 +106,41 @@
     <t>5.) Create an Entity Form Dynamic Renderer</t>
   </si>
   <si>
-    <t>6.) User Must Be Able to Login in with different Identity Providers(Database,Service,CRM).</t>
-  </si>
-  <si>
-    <t>7.) Create a UI Template for the MVC app solution</t>
-  </si>
-  <si>
     <t>3.) Create an Entity and Dynamic Renderer for Web Links</t>
   </si>
   <si>
     <t>2.) Create an ASP.NET Core solution</t>
+  </si>
+  <si>
+    <t>6.) Create a View Component for Lookups</t>
+  </si>
+  <si>
+    <t>7.) Create a View Component for Entity/List and SubGrid</t>
+  </si>
+  <si>
+    <t>8.) User Must Be Able to Login in with different Identity Providers(Database,Service,CRM).</t>
+  </si>
+  <si>
+    <t>9.) Administrator must be able to maintain User Entity</t>
+  </si>
+  <si>
+    <t>10.) Administrator must be able to maintain Roles Entity</t>
+  </si>
+  <si>
+    <t>11.) Administrator must be able to maintain Web Links Entity</t>
+  </si>
+  <si>
+    <t>Contributor</t>
+  </si>
+  <si>
+    <t>Rex</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,14 +171,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -170,7 +178,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,11 +194,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
       </patternFill>
     </fill>
     <fill>
@@ -223,13 +226,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -246,10 +248,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -259,9 +258,8 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
-    <cellStyle name="Good" xfId="3" builtinId="26"/>
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -541,27 +539,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="108" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -569,7 +571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -577,211 +579,301 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="96.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>30</v>
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>6</v>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>14</v>
+      <c r="B15" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>15</v>
+      <c r="A19" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>16</v>
+      <c r="A20" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>17</v>
+      <c r="A21" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="4" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>